<commit_message>
started data driven login tests using apache poi and testng
</commit_message>
<xml_diff>
--- a/src/data/loginDetails.xlsx
+++ b/src/data/loginDetails.xlsx
@@ -143,7 +143,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -177,10 +177,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>1</v>
+        <v>343</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>123</v>
+        <v>673</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed login tests with data driven framework
</commit_message>
<xml_diff>
--- a/src/data/loginDetails.xlsx
+++ b/src/data/loginDetails.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Username</t>
   </si>
@@ -33,6 +33,12 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>hi</t>
   </si>
 </sst>
 </file>
@@ -140,10 +146,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -176,11 +182,19 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>343</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>673</v>
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
addition of constants file to minimise errors in case of changes
</commit_message>
<xml_diff>
--- a/src/data/loginDetails.xlsx
+++ b/src/data/loginDetails.xlsx
@@ -146,10 +146,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -189,14 +189,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>32</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
refactored code, started signup parameterisation
</commit_message>
<xml_diff>
--- a/src/data/loginDetails.xlsx
+++ b/src/data/loginDetails.xlsx
@@ -5,17 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="222" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="232" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>Username</t>
   </si>
@@ -39,6 +40,51 @@
   </si>
   <si>
     <t>hi</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Email ID</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Set Password</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>person</t>
+  </si>
+  <si>
+    <t>person1</t>
+  </si>
+  <si>
+    <t>person1@email.com</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>person2</t>
+  </si>
+  <si>
+    <t>person2@gmail.com</t>
+  </si>
+  <si>
+    <t>somewhere</t>
   </si>
 </sst>
 </file>
@@ -48,7 +94,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -73,6 +119,24 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -120,12 +184,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -148,8 +224,8 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5:B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -198,4 +274,147 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.7244897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>1234</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>234</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>3423</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="person1@email.com"/>
+    <hyperlink ref="C4" r:id="rId2" display="person2@gmail.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
input data set for post and signup functionality
</commit_message>
<xml_diff>
--- a/src/data/loginDetails.xlsx
+++ b/src/data/loginDetails.xlsx
@@ -10,13 +10,14 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Username</t>
   </si>
@@ -66,9 +67,15 @@
     <t>Location</t>
   </si>
   <si>
+    <t>M</t>
+  </si>
+  <si>
     <t>person</t>
   </si>
   <si>
+    <t>F</t>
+  </si>
+  <si>
     <t>person1</t>
   </si>
   <si>
@@ -85,6 +92,33 @@
   </si>
   <si>
     <t>somewhere</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>The Title</t>
+  </si>
+  <si>
+    <t>Description of post</t>
+  </si>
+  <si>
+    <t>Peace Corps</t>
+  </si>
+  <si>
+    <t>New peace corps Post</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>@;':”</t>
+  </si>
+  <si>
+    <t>Characters</t>
   </si>
 </sst>
 </file>
@@ -94,7 +128,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -122,17 +156,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -184,7 +207,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -193,15 +216,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -284,7 +303,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -298,110 +317,119 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>16</v>
+      </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>18</v>
+      </c>
       <c r="B3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>1234</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>16</v>
+      </c>
       <c r="B4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>234</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>3423</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -417,4 +445,73 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>